<commit_message>
Allocations added to Google sheet
</commit_message>
<xml_diff>
--- a/output/data/alloc_final.xlsx
+++ b/output/data/alloc_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dannoble/Dropbox/1_Research/1_Manuscripts/In_Preparation/ecoevo_1000/output/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noble/Dropbox/1_Research/1_Manuscripts/In_Preparation/ecoevo_1000/output/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75C1E88-7F91-C044-9F6A-42D790DD2D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1A7141-657F-B843-829A-9DDE3C4455CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="31080" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46500" yWindow="500" windowWidth="18700" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,12 +479,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -499,11 +505,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -839,1108 +846,1108 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>4</v>
       </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
         <v>9</v>
       </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="E7" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D8" s="2">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>11</v>
       </c>
-      <c r="E9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="E9" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>11</v>
       </c>
-      <c r="E10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="E10" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>13</v>
       </c>
-      <c r="E11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="E11" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>14</v>
       </c>
-      <c r="E12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="E12" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>15</v>
       </c>
-      <c r="E13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="E13" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14">
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
         <v>17</v>
       </c>
-      <c r="E14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="E14" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>17</v>
       </c>
-      <c r="E15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="E15" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>18</v>
       </c>
-      <c r="E16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E16" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>18</v>
       </c>
-      <c r="E17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="E17" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>19</v>
       </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="E18" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>19</v>
       </c>
-      <c r="E19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="E19" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D20">
-        <v>20</v>
-      </c>
-      <c r="E20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="D20" s="2">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D21">
-        <v>20</v>
-      </c>
-      <c r="E21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="D21" s="2">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D22">
-        <v>20</v>
-      </c>
-      <c r="E22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="D22" s="2">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D23">
-        <v>20</v>
-      </c>
-      <c r="E23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="D23" s="2">
+        <v>20</v>
+      </c>
+      <c r="E23" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D24">
-        <v>20</v>
-      </c>
-      <c r="E24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D24" s="2">
+        <v>20</v>
+      </c>
+      <c r="E24" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D25">
-        <v>20</v>
-      </c>
-      <c r="E25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="D25" s="2">
+        <v>20</v>
+      </c>
+      <c r="E25" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D26">
-        <v>20</v>
-      </c>
-      <c r="E26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="D26" s="2">
+        <v>20</v>
+      </c>
+      <c r="E26" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D27">
-        <v>20</v>
-      </c>
-      <c r="E27">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="D27" s="2">
+        <v>20</v>
+      </c>
+      <c r="E27" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D28">
-        <v>20</v>
-      </c>
-      <c r="E28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="D28" s="2">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D29">
-        <v>20</v>
-      </c>
-      <c r="E29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="D29" s="2">
+        <v>20</v>
+      </c>
+      <c r="E29" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>21</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>21</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>21</v>
       </c>
-      <c r="E32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>22</v>
       </c>
-      <c r="E33">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="E33" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>22</v>
       </c>
-      <c r="E34">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="E34" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>22</v>
       </c>
-      <c r="E35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="E35" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>23</v>
       </c>
-      <c r="E36">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="E36" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>23</v>
       </c>
-      <c r="E37">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="E37" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>23</v>
       </c>
-      <c r="E38">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="E38" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <v>24</v>
       </c>
-      <c r="E39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="E39" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>24</v>
       </c>
-      <c r="E40">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="E40" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>24</v>
       </c>
-      <c r="E41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="E41" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>24</v>
       </c>
-      <c r="E42">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="E42" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="2">
         <v>25</v>
       </c>
-      <c r="E43">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="E43" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="2">
         <v>25</v>
       </c>
-      <c r="E44">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="E44" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="2">
         <v>25</v>
       </c>
-      <c r="E45">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="E45" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="2">
         <v>25</v>
       </c>
-      <c r="E46">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="E46" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="2">
         <v>25</v>
       </c>
-      <c r="E47">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="E47" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="2">
         <v>25</v>
       </c>
-      <c r="E48">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="E48" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="2">
         <v>25</v>
       </c>
-      <c r="E49">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="E49" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="2">
         <v>25</v>
       </c>
-      <c r="E50">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="E50" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="2">
         <v>25</v>
       </c>
-      <c r="E51">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="E51" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="2">
         <v>25</v>
       </c>
-      <c r="E52">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="E52" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="2">
         <v>25</v>
       </c>
-      <c r="E53">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="E53" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="2">
         <v>25</v>
       </c>
-      <c r="E54">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="E54" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="2">
         <v>25</v>
       </c>
-      <c r="E55">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="E55" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="2">
         <v>26</v>
       </c>
-      <c r="E56">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="E56" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="2">
         <v>26</v>
       </c>
-      <c r="E57">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="E57" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="2">
         <v>26</v>
       </c>
-      <c r="E58">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="E58" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="2">
         <v>27</v>
       </c>
-      <c r="E59">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="E59" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="2">
         <v>29</v>
       </c>
-      <c r="E60">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="E60" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="2">
         <v>48</v>
       </c>
-      <c r="E61">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="E61" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="64" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="65" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="66" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="2">
         <v>50</v>
       </c>
     </row>

</xml_diff>